<commit_message>
arreglos en insertBDAlumnos y crear profesor manualmente
</commit_message>
<xml_diff>
--- a/AlumnosImportacionMasiva.xlsx
+++ b/AlumnosImportacionMasiva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DayClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4739A67B-D8C2-4773-88AA-DBC1E19B62BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5ACB0-007F-4FEA-AE95-DE5F31E908DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>apellido</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
     <t>hernandez</t>
   </si>
   <si>
@@ -1309,6 +1306,9 @@
   </si>
   <si>
     <t>Laura</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1668,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1677,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1688,10 +1688,10 @@
         <v>83704</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,10 +1702,10 @@
         <v>89789</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1716,10 +1716,10 @@
         <v>80257</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1730,10 +1730,10 @@
         <v>61011</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1744,10 +1744,10 @@
         <v>85291</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1758,10 +1758,10 @@
         <v>72459</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1772,10 +1772,10 @@
         <v>76827</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1786,10 +1786,10 @@
         <v>68576</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1800,10 +1800,10 @@
         <v>59479</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1820,10 +1820,10 @@
         <v>73003</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1840,10 +1840,10 @@
         <v>51868</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1860,10 +1860,10 @@
         <v>78801</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1880,10 +1880,10 @@
         <v>54344</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1900,10 +1900,10 @@
         <v>54464</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1920,10 +1920,10 @@
         <v>45465</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1940,10 +1940,10 @@
         <v>75725</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1960,10 +1960,10 @@
         <v>85694</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1980,10 +1980,10 @@
         <v>85011</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>414</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2000,10 +2000,10 @@
         <v>65810</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2020,10 +2020,10 @@
         <v>44441</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -2040,10 +2040,10 @@
         <v>40222</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -2060,10 +2060,10 @@
         <v>83564</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2080,10 +2080,10 @@
         <v>73657</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2100,10 +2100,10 @@
         <v>81896</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2120,10 +2120,10 @@
         <v>44151</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2140,10 +2140,10 @@
         <v>82411</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2160,10 +2160,10 @@
         <v>82366</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2180,10 +2180,10 @@
         <v>50849</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2200,10 +2200,10 @@
         <v>45699</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2220,10 +2220,10 @@
         <v>58752</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2240,10 +2240,10 @@
         <v>81679</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2260,10 +2260,10 @@
         <v>61584</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2280,10 +2280,10 @@
         <v>83577</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2300,10 +2300,10 @@
         <v>69932</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2320,10 +2320,10 @@
         <v>44683</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -2340,10 +2340,10 @@
         <v>53241</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -2360,10 +2360,10 @@
         <v>42590</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2380,10 +2380,10 @@
         <v>75968</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>420</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2400,10 +2400,10 @@
         <v>67545</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -2420,10 +2420,10 @@
         <v>54662</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -2440,10 +2440,10 @@
         <v>65008</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -2460,10 +2460,10 @@
         <v>73675</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -2480,10 +2480,10 @@
         <v>88682</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2500,10 +2500,10 @@
         <v>87314</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2514,10 +2514,10 @@
         <v>67801</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2528,10 +2528,10 @@
         <v>70279</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2542,10 +2542,10 @@
         <v>89421</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2556,10 +2556,10 @@
         <v>45527</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2570,10 +2570,10 @@
         <v>70873</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2584,10 +2584,10 @@
         <v>61866</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2598,10 +2598,10 @@
         <v>76967</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2612,10 +2612,10 @@
         <v>56733</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2626,10 +2626,10 @@
         <v>57241</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2640,10 +2640,10 @@
         <v>62750</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2654,10 +2654,10 @@
         <v>69436</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2668,10 +2668,10 @@
         <v>85783</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2682,10 +2682,10 @@
         <v>48430</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2696,10 +2696,10 @@
         <v>89510</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2710,10 +2710,10 @@
         <v>88523</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2724,10 +2724,10 @@
         <v>51006</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2738,10 +2738,10 @@
         <v>86221</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2752,10 +2752,10 @@
         <v>54046</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2766,10 +2766,10 @@
         <v>74335</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2780,10 +2780,10 @@
         <v>63114</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2794,10 +2794,10 @@
         <v>66021</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2808,10 +2808,10 @@
         <v>40604</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,10 +2822,10 @@
         <v>53958</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2836,10 +2836,10 @@
         <v>48536</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2850,10 +2850,10 @@
         <v>44228</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2864,10 +2864,10 @@
         <v>69734</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2878,10 +2878,10 @@
         <v>57429</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2892,10 +2892,10 @@
         <v>73791</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2906,10 +2906,10 @@
         <v>87086</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2920,10 +2920,10 @@
         <v>80324</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2934,10 +2934,10 @@
         <v>68785</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2948,10 +2948,10 @@
         <v>57126</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2962,10 +2962,10 @@
         <v>40330</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2976,10 +2976,10 @@
         <v>69666</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2990,10 +2990,10 @@
         <v>72341</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3004,10 +3004,10 @@
         <v>62674</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,10 +3018,10 @@
         <v>50019</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E82" s="2"/>
     </row>
@@ -3033,10 +3033,10 @@
         <v>87104</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3047,10 +3047,10 @@
         <v>43096</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3061,10 +3061,10 @@
         <v>52979</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3075,10 +3075,10 @@
         <v>80480</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3089,10 +3089,10 @@
         <v>88033</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,10 +3103,10 @@
         <v>60823</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3117,10 +3117,10 @@
         <v>82923</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,10 +3131,10 @@
         <v>89861</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3145,10 +3145,10 @@
         <v>78263</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3159,10 +3159,10 @@
         <v>88904</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3173,10 +3173,10 @@
         <v>57231</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3187,10 +3187,10 @@
         <v>61221</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3201,10 +3201,10 @@
         <v>40049</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3215,10 +3215,10 @@
         <v>64138</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3229,10 +3229,10 @@
         <v>45154</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3243,10 +3243,10 @@
         <v>55486</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3257,10 +3257,10 @@
         <v>89351</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3271,10 +3271,10 @@
         <v>46006</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,10 +3285,10 @@
         <v>49312</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,10 +3299,10 @@
         <v>72481</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3313,10 +3313,10 @@
         <v>86212</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3327,10 +3327,10 @@
         <v>42674</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,10 +3341,10 @@
         <v>58586</v>
       </c>
       <c r="C105" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3355,10 +3355,10 @@
         <v>62837</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -3369,10 +3369,10 @@
         <v>50220</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3383,10 +3383,10 @@
         <v>79525</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3397,10 +3397,10 @@
         <v>54157</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3411,10 +3411,10 @@
         <v>89875</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,10 +3425,10 @@
         <v>70029</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3439,10 +3439,10 @@
         <v>70690</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,10 +3453,10 @@
         <v>68715</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3467,10 +3467,10 @@
         <v>43902</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3481,10 +3481,10 @@
         <v>46953</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3495,10 +3495,10 @@
         <v>57513</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,10 +3509,10 @@
         <v>74201</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3523,10 +3523,10 @@
         <v>77299</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3537,10 +3537,10 @@
         <v>68138</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3551,10 +3551,10 @@
         <v>43156</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3565,10 +3565,10 @@
         <v>44938</v>
       </c>
       <c r="C121" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3579,10 +3579,10 @@
         <v>89180</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3593,10 +3593,10 @@
         <v>73032</v>
       </c>
       <c r="C123" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3607,10 +3607,10 @@
         <v>87617</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3621,10 +3621,10 @@
         <v>68878</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3635,10 +3635,10 @@
         <v>59207</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3649,10 +3649,10 @@
         <v>80002</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3663,10 +3663,10 @@
         <v>83980</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,10 +3677,10 @@
         <v>47528</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3691,10 +3691,10 @@
         <v>53459</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,10 +3705,10 @@
         <v>60972</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3719,10 +3719,10 @@
         <v>48351</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3733,10 +3733,10 @@
         <v>70088</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3747,10 +3747,10 @@
         <v>53983</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3761,10 +3761,10 @@
         <v>82700</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3775,10 +3775,10 @@
         <v>81314</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3789,10 +3789,10 @@
         <v>66127</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3803,10 +3803,10 @@
         <v>52672</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3817,10 +3817,10 @@
         <v>82908</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3831,10 +3831,10 @@
         <v>42652</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3845,10 +3845,10 @@
         <v>44032</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3859,10 +3859,10 @@
         <v>81656</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,10 +3873,10 @@
         <v>49773</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,10 +3887,10 @@
         <v>59702</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,10 +3901,10 @@
         <v>81363</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3915,10 +3915,10 @@
         <v>71031</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,10 +3929,10 @@
         <v>47299</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3943,10 +3943,10 @@
         <v>80383</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,10 +3957,10 @@
         <v>87563</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,10 +3971,10 @@
         <v>45399</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,10 +3985,10 @@
         <v>63387</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3999,10 +3999,10 @@
         <v>52179</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4013,10 +4013,10 @@
         <v>80228</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4027,10 +4027,10 @@
         <v>78625</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4041,10 +4041,10 @@
         <v>80882</v>
       </c>
       <c r="C155" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,10 +4055,10 @@
         <v>64039</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4069,10 +4069,10 @@
         <v>77545</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,10 +4083,10 @@
         <v>58351</v>
       </c>
       <c r="C158" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4097,10 +4097,10 @@
         <v>80620</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4111,10 +4111,10 @@
         <v>63535</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4125,10 +4125,10 @@
         <v>58539</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4139,10 +4139,10 @@
         <v>45396</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4153,10 +4153,10 @@
         <v>48843</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,10 +4167,10 @@
         <v>46594</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,10 +4181,10 @@
         <v>59978</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4195,10 +4195,10 @@
         <v>67133</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4209,10 +4209,10 @@
         <v>63167</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4223,10 +4223,10 @@
         <v>53384</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4237,10 +4237,10 @@
         <v>71107</v>
       </c>
       <c r="C169" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,10 +4251,10 @@
         <v>50309</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4265,10 +4265,10 @@
         <v>56889</v>
       </c>
       <c r="C171" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4279,10 +4279,10 @@
         <v>41400</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4293,10 +4293,10 @@
         <v>68788</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4307,10 +4307,10 @@
         <v>81087</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>87457</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4335,10 +4335,10 @@
         <v>69488</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4349,10 +4349,10 @@
         <v>58354</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4363,10 +4363,10 @@
         <v>51420</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4377,10 +4377,10 @@
         <v>47281</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4391,10 +4391,10 @@
         <v>53352</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4405,10 +4405,10 @@
         <v>73283</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,10 +4419,10 @@
         <v>61437</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4433,10 +4433,10 @@
         <v>75287</v>
       </c>
       <c r="C183" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D183" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -4447,10 +4447,10 @@
         <v>71969</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,10 +4461,10 @@
         <v>51491</v>
       </c>
       <c r="C185" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D185" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="D185" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -4475,10 +4475,10 @@
         <v>71707</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4489,10 +4489,10 @@
         <v>58815</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4503,10 +4503,10 @@
         <v>54834</v>
       </c>
       <c r="C188" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D188" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4517,10 +4517,10 @@
         <v>59714</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4531,10 +4531,10 @@
         <v>49703</v>
       </c>
       <c r="C190" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D190" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -4545,10 +4545,10 @@
         <v>60450</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -4559,10 +4559,10 @@
         <v>55390</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4573,10 +4573,10 @@
         <v>54944</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -4587,10 +4587,10 @@
         <v>41414</v>
       </c>
       <c r="C194" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D194" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4601,10 +4601,10 @@
         <v>47936</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -4615,10 +4615,10 @@
         <v>73236</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4629,10 +4629,10 @@
         <v>41350</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4643,10 +4643,10 @@
         <v>46100</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4657,10 +4657,10 @@
         <v>78998</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,10 +4671,10 @@
         <v>54416</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,10 +4685,10 @@
         <v>73629</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4699,10 +4699,10 @@
         <v>43487</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4713,10 +4713,10 @@
         <v>70125</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,10 +4727,10 @@
         <v>52551</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,10 +4741,10 @@
         <v>56060</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,10 +4755,10 @@
         <v>79979</v>
       </c>
       <c r="C206" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D206" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="D206" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4769,10 +4769,10 @@
         <v>44872</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -4783,10 +4783,10 @@
         <v>74106</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4797,10 +4797,10 @@
         <v>85361</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4811,10 +4811,10 @@
         <v>57084</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4825,10 +4825,10 @@
         <v>59091</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -4839,10 +4839,10 @@
         <v>67388</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -4853,10 +4853,10 @@
         <v>89984</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -4867,10 +4867,10 @@
         <v>48906</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,10 +4881,10 @@
         <v>45377</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -4895,10 +4895,10 @@
         <v>84933</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -4909,10 +4909,10 @@
         <v>68781</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -4923,10 +4923,10 @@
         <v>68143</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,10 +4937,10 @@
         <v>71397</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -4951,10 +4951,10 @@
         <v>52926</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -4965,10 +4965,10 @@
         <v>80241</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,10 +4979,10 @@
         <v>57567</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -4993,10 +4993,10 @@
         <v>73358</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5007,10 +5007,10 @@
         <v>76877</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,10 +5021,10 @@
         <v>41867</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5035,10 +5035,10 @@
         <v>73682</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5049,10 +5049,10 @@
         <v>87270</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,10 +5063,10 @@
         <v>79314</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -5077,10 +5077,10 @@
         <v>49596</v>
       </c>
       <c r="C229" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D229" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="D229" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,10 +5091,10 @@
         <v>87607</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,10 +5105,10 @@
         <v>72036</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>